<commit_message>
Cleaning horsepower to float
</commit_message>
<xml_diff>
--- a/EMD Locomotives.xlsx
+++ b/EMD Locomotives.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ds57534\Documents\GitHub\Web-Scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325EE258-4DB3-4678-BC80-268BCB8190FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C27ED0-E0F8-40D5-BB3A-5A17745FD16D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{F910C9BC-1477-402A-AE45-760ECDD26B64}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="124">
   <si>
     <t>GP7</t>
   </si>
@@ -45,9 +45,6 @@
     <t>2,729 A units</t>
   </si>
   <si>
-    <t>1,500 hp</t>
-  </si>
-  <si>
     <t>GP9</t>
   </si>
   <si>
@@ -57,9 +54,6 @@
     <t>4,272 A units</t>
   </si>
   <si>
-    <t>1,750 hp</t>
-  </si>
-  <si>
     <t>GP15-1</t>
   </si>
   <si>
@@ -81,18 +75,12 @@
     <t>1959–1963</t>
   </si>
   <si>
-    <t>1,800 hp</t>
-  </si>
-  <si>
     <t>GP20</t>
   </si>
   <si>
     <t>1959–1962</t>
   </si>
   <si>
-    <t>2,000 hp</t>
-  </si>
-  <si>
     <t>GP28</t>
   </si>
   <si>
@@ -108,18 +96,12 @@
     <t>908 A units</t>
   </si>
   <si>
-    <t>2,250 hp</t>
-  </si>
-  <si>
     <t>GP35</t>
   </si>
   <si>
     <t>1963–1966</t>
   </si>
   <si>
-    <t>2,500 hp</t>
-  </si>
-  <si>
     <t>GP38</t>
   </si>
   <si>
@@ -153,18 +135,12 @@
     <t>1969–1970</t>
   </si>
   <si>
-    <t>2,300 hp</t>
-  </si>
-  <si>
     <t>GP39DC</t>
   </si>
   <si>
     <t>GP39X</t>
   </si>
   <si>
-    <t>2,600 hp</t>
-  </si>
-  <si>
     <t>GP39-2</t>
   </si>
   <si>
@@ -177,9 +153,6 @@
     <t>1965–1971</t>
   </si>
   <si>
-    <t>3,000 hp</t>
-  </si>
-  <si>
     <t>GP40P</t>
   </si>
   <si>
@@ -195,9 +168,6 @@
     <t>1977–1978</t>
   </si>
   <si>
-    <t>3,500 hp</t>
-  </si>
-  <si>
     <t>GP40-2</t>
   </si>
   <si>
@@ -207,9 +177,6 @@
     <t>1983–1985</t>
   </si>
   <si>
-    <t>2,800 hp</t>
-  </si>
-  <si>
     <t>GP50</t>
   </si>
   <si>
@@ -231,18 +198,12 @@
     <t>294 A units</t>
   </si>
   <si>
-    <t>3,800 hp</t>
-  </si>
-  <si>
     <t>GP60M</t>
   </si>
   <si>
     <t>EMC pre – SC</t>
   </si>
   <si>
-    <t>600 hp</t>
-  </si>
-  <si>
     <t>SC</t>
   </si>
   <si>
@@ -252,9 +213,6 @@
     <t>Model 90</t>
   </si>
   <si>
-    <t>900 hp</t>
-  </si>
-  <si>
     <t>SW</t>
   </si>
   <si>
@@ -291,9 +249,6 @@
     <t>1939–1949</t>
   </si>
   <si>
-    <t>1,000 hp</t>
-  </si>
-  <si>
     <t>NW4</t>
   </si>
   <si>
@@ -303,9 +258,6 @@
     <t>TR1</t>
   </si>
   <si>
-    <t>2,700 hp</t>
-  </si>
-  <si>
     <t>TR2</t>
   </si>
   <si>
@@ -321,9 +273,6 @@
     <t>1950–1951</t>
   </si>
   <si>
-    <t>2,400 hp</t>
-  </si>
-  <si>
     <t>TR5</t>
   </si>
   <si>
@@ -336,9 +285,6 @@
     <t>1950–1953</t>
   </si>
   <si>
-    <t>1,600 hp</t>
-  </si>
-  <si>
     <t>SW1</t>
   </si>
   <si>
@@ -351,18 +297,12 @@
     <t>1949–1951</t>
   </si>
   <si>
-    <t>1,200 hp</t>
-  </si>
-  <si>
     <t>SW8</t>
   </si>
   <si>
     <t>1950–1954</t>
   </si>
   <si>
-    <t>800 hp</t>
-  </si>
-  <si>
     <t>DH2</t>
   </si>
   <si>
@@ -441,9 +381,6 @@
     <t>RS1325</t>
   </si>
   <si>
-    <t>1,325 hp</t>
-  </si>
-  <si>
     <t>GMD1</t>
   </si>
   <si>
@@ -456,9 +393,6 @@
     <t>1940–1943</t>
   </si>
   <si>
-    <t>300 hp</t>
-  </si>
-  <si>
     <t>DH1</t>
   </si>
   <si>
@@ -472,9 +406,6 @@
   </si>
   <si>
     <t>Power Output</t>
-  </si>
-  <si>
-    <t>340 hp</t>
   </si>
 </sst>
 </file>
@@ -510,8 +441,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -828,29 +760,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76643D5-62EC-4DF3-85F2-7E4F76A9A9A4}">
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="B1" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="C1" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
       <c r="D1" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B2">
         <v>1935</v>
@@ -858,27 +790,27 @@
       <c r="C2">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
-        <v>68</v>
+      <c r="D2">
+        <v>600</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C3">
         <v>43</v>
       </c>
-      <c r="D3" t="s">
-        <v>68</v>
+      <c r="D3">
+        <v>600</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B4">
         <v>1935</v>
@@ -886,41 +818,41 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
-        <v>72</v>
+      <c r="D4">
+        <v>900</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C5">
         <v>76</v>
       </c>
-      <c r="D5" t="s">
-        <v>68</v>
+      <c r="D5">
+        <v>600</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
-        <v>72</v>
+      <c r="D6">
+        <v>900</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B7">
         <v>1937</v>
@@ -928,13 +860,13 @@
       <c r="C7">
         <v>5</v>
       </c>
-      <c r="D7" t="s">
-        <v>72</v>
+      <c r="D7">
+        <v>900</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B8">
         <v>1937</v>
@@ -942,13 +874,13 @@
       <c r="C8">
         <v>2</v>
       </c>
-      <c r="D8" t="s">
-        <v>72</v>
+      <c r="D8">
+        <v>900</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B9">
         <v>1936</v>
@@ -956,41 +888,41 @@
       <c r="C9">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
-        <v>15</v>
+      <c r="D9" s="1">
+        <v>1800</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C10">
         <v>8</v>
       </c>
-      <c r="D10" t="s">
-        <v>72</v>
+      <c r="D10">
+        <v>900</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C11">
         <v>27</v>
       </c>
-      <c r="D11" t="s">
-        <v>72</v>
+      <c r="D11">
+        <v>900</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B12">
         <v>1938</v>
@@ -998,27 +930,27 @@
       <c r="C12">
         <v>3</v>
       </c>
-      <c r="D12" t="s">
-        <v>72</v>
+      <c r="D12">
+        <v>900</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C13">
         <v>1145</v>
       </c>
-      <c r="D13" t="s">
-        <v>85</v>
+      <c r="D13" s="1">
+        <v>1000</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B14">
         <v>1938</v>
@@ -1026,55 +958,55 @@
       <c r="C14">
         <v>2</v>
       </c>
-      <c r="D14" t="s">
-        <v>72</v>
+      <c r="D14">
+        <v>900</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
       <c r="B15" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="C15">
         <v>661</v>
       </c>
-      <c r="D15" t="s">
-        <v>68</v>
+      <c r="D15">
+        <v>600</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="B16" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
       <c r="C16">
         <v>489</v>
       </c>
-      <c r="D16" t="s">
-        <v>105</v>
+      <c r="D16" s="1">
+        <v>1200</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="C17">
         <v>373</v>
       </c>
-      <c r="D17" t="s">
-        <v>108</v>
+      <c r="D17">
+        <v>800</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="B18">
         <v>1953</v>
@@ -1082,139 +1014,139 @@
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="D18" t="s">
-        <v>108</v>
+      <c r="D18">
+        <v>800</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="C19">
         <v>815</v>
       </c>
-      <c r="D19" t="s">
-        <v>105</v>
+      <c r="D19" s="1">
+        <v>1200</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="B20" t="s">
-        <v>112</v>
+        <v>92</v>
       </c>
       <c r="C20">
         <v>75</v>
       </c>
-      <c r="D20" t="s">
-        <v>85</v>
+      <c r="D20" s="1">
+        <v>1000</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>113</v>
+        <v>93</v>
       </c>
       <c r="B21" t="s">
-        <v>114</v>
+        <v>94</v>
       </c>
       <c r="C21">
         <v>112</v>
       </c>
-      <c r="D21" t="s">
-        <v>85</v>
+      <c r="D21" s="1">
+        <v>1000</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="B22" t="s">
-        <v>116</v>
+        <v>96</v>
       </c>
       <c r="C22">
         <v>15</v>
       </c>
-      <c r="D22" t="s">
-        <v>68</v>
+      <c r="D22">
+        <v>600</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>117</v>
+        <v>97</v>
       </c>
       <c r="B23" t="s">
-        <v>118</v>
+        <v>98</v>
       </c>
       <c r="C23">
         <v>371</v>
       </c>
-      <c r="D23" t="s">
-        <v>72</v>
+      <c r="D23">
+        <v>900</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="B24" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="C24">
         <v>119</v>
       </c>
-      <c r="D24" t="s">
-        <v>85</v>
+      <c r="D24" s="1">
+        <v>1000</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="B25" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="C25">
         <v>230</v>
       </c>
-      <c r="D25" t="s">
-        <v>85</v>
+      <c r="D25" s="1">
+        <v>1000</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>123</v>
+        <v>103</v>
       </c>
       <c r="B26" t="s">
-        <v>124</v>
+        <v>104</v>
       </c>
       <c r="C26">
         <v>1056</v>
       </c>
-      <c r="D26" t="s">
-        <v>105</v>
+      <c r="D26" s="1">
+        <v>1200</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
-        <v>126</v>
+        <v>106</v>
       </c>
       <c r="C27">
         <v>808</v>
       </c>
-      <c r="D27" t="s">
-        <v>3</v>
+      <c r="D27" s="1">
+        <v>1500</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>127</v>
+        <v>107</v>
       </c>
       <c r="B28">
         <v>1973</v>
@@ -1222,55 +1154,55 @@
       <c r="C28">
         <v>60</v>
       </c>
-      <c r="D28" t="s">
-        <v>3</v>
+      <c r="D28" s="1">
+        <v>1500</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>128</v>
+        <v>108</v>
       </c>
       <c r="B29" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C29">
         <v>351</v>
       </c>
-      <c r="D29" t="s">
-        <v>3</v>
+      <c r="D29" s="1">
+        <v>1500</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>130</v>
+        <v>110</v>
       </c>
       <c r="B30" t="s">
-        <v>131</v>
+        <v>111</v>
       </c>
       <c r="C30">
         <v>246</v>
       </c>
-      <c r="D30" t="s">
-        <v>3</v>
+      <c r="D30" s="1">
+        <v>1500</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>132</v>
+        <v>112</v>
       </c>
       <c r="B31" t="s">
-        <v>133</v>
+        <v>113</v>
       </c>
       <c r="C31">
         <v>43</v>
       </c>
-      <c r="D31" t="s">
-        <v>3</v>
+      <c r="D31" s="1">
+        <v>1500</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>134</v>
+        <v>114</v>
       </c>
       <c r="B32">
         <v>1960</v>
@@ -1278,22 +1210,22 @@
       <c r="C32">
         <v>2</v>
       </c>
-      <c r="D32" t="s">
-        <v>135</v>
+      <c r="D32" s="1">
+        <v>1325</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="C33">
         <v>101</v>
       </c>
-      <c r="D33" t="s">
-        <v>105</v>
+      <c r="D33" s="1">
+        <v>1200</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1306,41 +1238,41 @@
       <c r="C34" t="s">
         <v>2</v>
       </c>
-      <c r="D34" t="s">
-        <v>3</v>
+      <c r="D34" s="1">
+        <v>1500</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35" t="s">
         <v>4</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>5</v>
       </c>
-      <c r="C35" t="s">
-        <v>6</v>
-      </c>
-      <c r="D35" t="s">
-        <v>7</v>
+      <c r="D35" s="1">
+        <v>1750</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C36">
         <v>310</v>
       </c>
-      <c r="D36" t="s">
-        <v>3</v>
+      <c r="D36" s="1">
+        <v>1500</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B37">
         <v>1982</v>
@@ -1348,175 +1280,175 @@
       <c r="C37">
         <v>34</v>
       </c>
-      <c r="D37" t="s">
-        <v>3</v>
+      <c r="D37" s="1">
+        <v>1500</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C38">
         <v>28</v>
       </c>
-      <c r="D38" t="s">
-        <v>3</v>
+      <c r="D38" s="1">
+        <v>1500</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B39" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C39">
         <v>405</v>
       </c>
-      <c r="D39" t="s">
-        <v>15</v>
+      <c r="D39" s="1">
+        <v>1800</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B40" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C40">
         <v>260</v>
       </c>
-      <c r="D40" t="s">
-        <v>18</v>
+      <c r="D40" s="1">
+        <v>2000</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B41" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C41">
         <v>31</v>
       </c>
-      <c r="D41" t="s">
-        <v>15</v>
+      <c r="D41" s="1">
+        <v>1800</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B42" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C42" t="s">
-        <v>23</v>
-      </c>
-      <c r="D42" t="s">
-        <v>24</v>
+        <v>19</v>
+      </c>
+      <c r="D42" s="1">
+        <v>2250</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B43" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C43">
         <v>1334</v>
       </c>
-      <c r="D43" t="s">
-        <v>27</v>
+      <c r="D43" s="1">
+        <v>2500</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B44" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C44">
         <v>706</v>
       </c>
-      <c r="D44" t="s">
-        <v>18</v>
+      <c r="D44" s="1">
+        <v>2000</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B45" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C45">
         <v>261</v>
       </c>
-      <c r="D45" t="s">
-        <v>18</v>
+      <c r="D45" s="1">
+        <v>2000</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B46" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C46">
         <v>2213</v>
       </c>
-      <c r="D46" t="s">
-        <v>18</v>
+      <c r="D46" s="1">
+        <v>2000</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>34</v>
-      </c>
-      <c r="D47" t="s">
-        <v>18</v>
+        <v>28</v>
+      </c>
+      <c r="D47" s="1">
+        <v>2000</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B48" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C48">
         <v>51</v>
       </c>
-      <c r="D48" t="s">
-        <v>18</v>
+      <c r="D48" s="1">
+        <v>2000</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B49" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C49">
         <v>23</v>
       </c>
-      <c r="D49" t="s">
-        <v>39</v>
+      <c r="D49" s="1">
+        <v>2300</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B50">
         <v>1970</v>
@@ -1524,13 +1456,13 @@
       <c r="C50">
         <v>2</v>
       </c>
-      <c r="D50" t="s">
-        <v>39</v>
+      <c r="D50" s="1">
+        <v>2300</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B51">
         <v>1980</v>
@@ -1538,41 +1470,41 @@
       <c r="C51">
         <v>6</v>
       </c>
-      <c r="D51" t="s">
-        <v>42</v>
+      <c r="D51" s="1">
+        <v>2600</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B52" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C52">
         <v>239</v>
       </c>
-      <c r="D52" t="s">
-        <v>39</v>
+      <c r="D52" s="1">
+        <v>2300</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B53" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C53">
         <v>1221</v>
       </c>
-      <c r="D53" t="s">
-        <v>47</v>
+      <c r="D53" s="1">
+        <v>3000</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B54">
         <v>1968</v>
@@ -1580,13 +1512,13 @@
       <c r="C54">
         <v>13</v>
       </c>
-      <c r="D54" t="s">
-        <v>47</v>
+      <c r="D54" s="1">
+        <v>3000</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B55">
         <v>1974</v>
@@ -1594,13 +1526,13 @@
       <c r="C55">
         <v>3</v>
       </c>
-      <c r="D55" t="s">
-        <v>47</v>
+      <c r="D55" s="1">
+        <v>3000</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B56">
         <v>1966</v>
@@ -1608,97 +1540,97 @@
       <c r="C56">
         <v>8</v>
       </c>
-      <c r="D56" t="s">
-        <v>47</v>
+      <c r="D56" s="1">
+        <v>3000</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B57" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="C57">
         <v>23</v>
       </c>
-      <c r="D57" t="s">
-        <v>53</v>
+      <c r="D57" s="1">
+        <v>3500</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B58" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C58">
         <v>1140</v>
       </c>
-      <c r="D58" t="s">
-        <v>47</v>
+      <c r="D58" s="1">
+        <v>3000</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B59" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="C59">
         <v>9</v>
       </c>
-      <c r="D59" t="s">
-        <v>57</v>
+      <c r="D59" s="1">
+        <v>2800</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="B60" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="C60">
         <v>278</v>
       </c>
-      <c r="D60" t="s">
-        <v>53</v>
+      <c r="D60" s="1">
+        <v>3500</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="B61" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C61">
         <v>36</v>
       </c>
-      <c r="D61" t="s">
-        <v>47</v>
+      <c r="D61" s="1">
+        <v>3000</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B62" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="C62" t="s">
-        <v>64</v>
-      </c>
-      <c r="D62" t="s">
-        <v>65</v>
+        <v>53</v>
+      </c>
+      <c r="D62" s="1">
+        <v>3800</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B63">
         <v>1990</v>
@@ -1706,27 +1638,27 @@
       <c r="C63">
         <v>63</v>
       </c>
-      <c r="D63" t="s">
-        <v>65</v>
+      <c r="D63" s="1">
+        <v>3800</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="B64" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="C64">
         <v>11</v>
       </c>
-      <c r="D64" t="s">
-        <v>140</v>
+      <c r="D64">
+        <v>300</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="B65">
         <v>1951</v>
@@ -1734,13 +1666,13 @@
       <c r="C65">
         <v>33</v>
       </c>
-      <c r="D65" t="s">
-        <v>146</v>
+      <c r="D65">
+        <v>340</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B66">
         <v>1940</v>
@@ -1748,13 +1680,13 @@
       <c r="C66">
         <v>3</v>
       </c>
-      <c r="D66" t="s">
-        <v>18</v>
+      <c r="D66" s="1">
+        <v>2000</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B67">
         <v>1941</v>
@@ -1762,27 +1694,27 @@
       <c r="C67">
         <v>2</v>
       </c>
-      <c r="D67" t="s">
-        <v>89</v>
+      <c r="D67" s="1">
+        <v>2700</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B68" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="C68">
         <v>36</v>
       </c>
-      <c r="D68" t="s">
-        <v>18</v>
+      <c r="D68" s="1">
+        <v>2000</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B69">
         <v>1949</v>
@@ -1790,50 +1722,50 @@
       <c r="C69">
         <v>2</v>
       </c>
-      <c r="D69" t="s">
-        <v>47</v>
+      <c r="D69" s="1">
+        <v>3000</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B70" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="C70">
         <v>15</v>
       </c>
-      <c r="D70" t="s">
-        <v>95</v>
+      <c r="D70" s="1">
+        <v>2400</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="B71">
         <v>1951</v>
       </c>
       <c r="C71" t="s">
-        <v>97</v>
-      </c>
-      <c r="D71" t="s">
-        <v>95</v>
+        <v>80</v>
+      </c>
+      <c r="D71" s="1">
+        <v>2400</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B72" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="C72">
         <v>12</v>
       </c>
-      <c r="D72" t="s">
-        <v>100</v>
+      <c r="D72" s="1">
+        <v>1600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Horsepower assignment script functionality achieved to dieselshop locomotive list
</commit_message>
<xml_diff>
--- a/EMD Locomotives.xlsx
+++ b/EMD Locomotives.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ds57534\Documents\GitHub\Web-Scraping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73C27ED0-E0F8-40D5-BB3A-5A17745FD16D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4501954-653E-4357-A759-F5302840E6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{F910C9BC-1477-402A-AE45-760ECDD26B64}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="280">
   <si>
     <t>GP7</t>
   </si>
@@ -406,6 +406,474 @@
   </si>
   <si>
     <t>Power Output</t>
+  </si>
+  <si>
+    <t>GMDH-1</t>
+  </si>
+  <si>
+    <t>1956–1959</t>
+  </si>
+  <si>
+    <t>GMDH-3</t>
+  </si>
+  <si>
+    <t>BL1</t>
+  </si>
+  <si>
+    <t>BL2</t>
+  </si>
+  <si>
+    <t>1948–1949</t>
+  </si>
+  <si>
+    <t>BL20-2</t>
+  </si>
+  <si>
+    <t>GP15D</t>
+  </si>
+  <si>
+    <t>2000–2001</t>
+  </si>
+  <si>
+    <t>GP20D</t>
+  </si>
+  <si>
+    <t>SD7</t>
+  </si>
+  <si>
+    <t>1952–1953</t>
+  </si>
+  <si>
+    <t>SD9</t>
+  </si>
+  <si>
+    <t>1954–1959</t>
+  </si>
+  <si>
+    <t>SD18</t>
+  </si>
+  <si>
+    <t>1960–1963</t>
+  </si>
+  <si>
+    <t>SD24</t>
+  </si>
+  <si>
+    <t>1958–1963</t>
+  </si>
+  <si>
+    <t>SD28</t>
+  </si>
+  <si>
+    <t>1965-1966</t>
+  </si>
+  <si>
+    <t>SD35</t>
+  </si>
+  <si>
+    <t>1964–1966</t>
+  </si>
+  <si>
+    <t>SDP35</t>
+  </si>
+  <si>
+    <t>SD38</t>
+  </si>
+  <si>
+    <t>1967–1971</t>
+  </si>
+  <si>
+    <t>SD38AC</t>
+  </si>
+  <si>
+    <t>SD38-2</t>
+  </si>
+  <si>
+    <t>1972–1979</t>
+  </si>
+  <si>
+    <t>SDP38</t>
+  </si>
+  <si>
+    <t>SD39</t>
+  </si>
+  <si>
+    <t>1968–1970</t>
+  </si>
+  <si>
+    <t>SDL39</t>
+  </si>
+  <si>
+    <t>1969–1972</t>
+  </si>
+  <si>
+    <t>SD40X</t>
+  </si>
+  <si>
+    <t>SD40</t>
+  </si>
+  <si>
+    <t>SD40A</t>
+  </si>
+  <si>
+    <t>SDP40</t>
+  </si>
+  <si>
+    <t>1966–1970</t>
+  </si>
+  <si>
+    <t>SD40T-2</t>
+  </si>
+  <si>
+    <t>SD40-2</t>
+  </si>
+  <si>
+    <t>1972–1989</t>
+  </si>
+  <si>
+    <t>SD40-2W</t>
+  </si>
+  <si>
+    <t>1975–1980</t>
+  </si>
+  <si>
+    <t>SD40-2S</t>
+  </si>
+  <si>
+    <t>1978–1980</t>
+  </si>
+  <si>
+    <t>SD45</t>
+  </si>
+  <si>
+    <t>SD45X</t>
+  </si>
+  <si>
+    <t>SDP45</t>
+  </si>
+  <si>
+    <t>1967–1970</t>
+  </si>
+  <si>
+    <t>SD45T-2</t>
+  </si>
+  <si>
+    <t>1972–1975</t>
+  </si>
+  <si>
+    <t>SD45-2</t>
+  </si>
+  <si>
+    <t>1972–1974</t>
+  </si>
+  <si>
+    <t>SD50</t>
+  </si>
+  <si>
+    <t>SD50S</t>
+  </si>
+  <si>
+    <t>SD60</t>
+  </si>
+  <si>
+    <t>1984–1991</t>
+  </si>
+  <si>
+    <t>SD60I</t>
+  </si>
+  <si>
+    <t>1993–1995</t>
+  </si>
+  <si>
+    <t>SD60M</t>
+  </si>
+  <si>
+    <t>1989–1993</t>
+  </si>
+  <si>
+    <t>SD60MAC</t>
+  </si>
+  <si>
+    <t>1991–1992</t>
+  </si>
+  <si>
+    <t>SD70</t>
+  </si>
+  <si>
+    <t>1992–1999</t>
+  </si>
+  <si>
+    <t>SD70I</t>
+  </si>
+  <si>
+    <t>SD70ACe</t>
+  </si>
+  <si>
+    <t>2003-</t>
+  </si>
+  <si>
+    <t>SD70ACS</t>
+  </si>
+  <si>
+    <t>2009–</t>
+  </si>
+  <si>
+    <t>SD70M</t>
+  </si>
+  <si>
+    <t>1992–2004</t>
+  </si>
+  <si>
+    <t>SD70M-2</t>
+  </si>
+  <si>
+    <t>2004–</t>
+  </si>
+  <si>
+    <t>SD70MAC</t>
+  </si>
+  <si>
+    <t>1993–2004</t>
+  </si>
+  <si>
+    <t>SD75M</t>
+  </si>
+  <si>
+    <t>1995–1996</t>
+  </si>
+  <si>
+    <t>SD75I</t>
+  </si>
+  <si>
+    <t>1996–1999</t>
+  </si>
+  <si>
+    <t>SD80MAC</t>
+  </si>
+  <si>
+    <t>SD89MAC</t>
+  </si>
+  <si>
+    <t>SD90MAC</t>
+  </si>
+  <si>
+    <t>1995–2005</t>
+  </si>
+  <si>
+    <t>SD70ACe-T4</t>
+  </si>
+  <si>
+    <t>2015-</t>
+  </si>
+  <si>
+    <t>DD35</t>
+  </si>
+  <si>
+    <t>1963–1964</t>
+  </si>
+  <si>
+    <t>DD35A</t>
+  </si>
+  <si>
+    <t>DDA40X</t>
+  </si>
+  <si>
+    <t>1969–1971</t>
+  </si>
+  <si>
+    <t>FP45</t>
+  </si>
+  <si>
+    <t>F45</t>
+  </si>
+  <si>
+    <t>1968–1971</t>
+  </si>
+  <si>
+    <t>SDP40F</t>
+  </si>
+  <si>
+    <t>F40C</t>
+  </si>
+  <si>
+    <t>F40PH</t>
+  </si>
+  <si>
+    <t>1975–1988</t>
+  </si>
+  <si>
+    <t>F40PHR</t>
+  </si>
+  <si>
+    <t>1977–1985</t>
+  </si>
+  <si>
+    <t>F40PH-2M</t>
+  </si>
+  <si>
+    <t>1982–1985</t>
+  </si>
+  <si>
+    <t>F40PH-2</t>
+  </si>
+  <si>
+    <t>F40PH-2C</t>
+  </si>
+  <si>
+    <t>1987–1988</t>
+  </si>
+  <si>
+    <t>F40PHM-2</t>
+  </si>
+  <si>
+    <t>SD40-2F</t>
+  </si>
+  <si>
+    <t>SD50F</t>
+  </si>
+  <si>
+    <t>1985–1987</t>
+  </si>
+  <si>
+    <t>SD60F</t>
+  </si>
+  <si>
+    <t>F59PH</t>
+  </si>
+  <si>
+    <t>1988–1994</t>
+  </si>
+  <si>
+    <t>F59PHI</t>
+  </si>
+  <si>
+    <t>1994–2001</t>
+  </si>
+  <si>
+    <t>F69PHAC</t>
+  </si>
+  <si>
+    <t>DE30AC,</t>
+  </si>
+  <si>
+    <t>DM30AC</t>
+  </si>
+  <si>
+    <t>1997–1999</t>
+  </si>
+  <si>
+    <t>F125</t>
+  </si>
+  <si>
+    <t>2015-2021</t>
+  </si>
+  <si>
+    <t>1997-1999</t>
+  </si>
+  <si>
+    <t>CF7</t>
+  </si>
+  <si>
+    <t>1970–1978</t>
+  </si>
+  <si>
+    <t>GP15C</t>
+  </si>
+  <si>
+    <t>1990–1991</t>
+  </si>
+  <si>
+    <t>GP16</t>
+  </si>
+  <si>
+    <t>1979–1982</t>
+  </si>
+  <si>
+    <t>G18AR</t>
+  </si>
+  <si>
+    <t>1979–1981</t>
+  </si>
+  <si>
+    <t>G22AR</t>
+  </si>
+  <si>
+    <t>1977–1982</t>
+  </si>
+  <si>
+    <t>G22CR</t>
+  </si>
+  <si>
+    <t>1998–2001</t>
+  </si>
+  <si>
+    <t>GP30C</t>
+  </si>
+  <si>
+    <t>GP38H-3</t>
+  </si>
+  <si>
+    <t>2004-2005</t>
+  </si>
+  <si>
+    <t>GP39H-2</t>
+  </si>
+  <si>
+    <t>GP40FH-2</t>
+  </si>
+  <si>
+    <t>1987-1990</t>
+  </si>
+  <si>
+    <t>GP40PH-2</t>
+  </si>
+  <si>
+    <t>1991-1994</t>
+  </si>
+  <si>
+    <t>GP40WH-2</t>
+  </si>
+  <si>
+    <t>SD20</t>
+  </si>
+  <si>
+    <t>SD26</t>
+  </si>
+  <si>
+    <t>1973–1978</t>
+  </si>
+  <si>
+    <t>SD39-2M</t>
+  </si>
+  <si>
+    <t>GP22ECO</t>
+  </si>
+  <si>
+    <t>SD22ECO</t>
+  </si>
+  <si>
+    <t>SD32ECO</t>
+  </si>
+  <si>
+    <t>GP20C-ECO</t>
+  </si>
+  <si>
+    <t>SD30C-ECO</t>
+  </si>
+  <si>
+    <t>2013-2017</t>
+  </si>
+  <si>
+    <t>SD70MACH</t>
+  </si>
+  <si>
+    <t>2022-</t>
+  </si>
+  <si>
+    <t>J16CW/AC</t>
+  </si>
+  <si>
+    <t>1984-1985</t>
   </si>
 </sst>
 </file>
@@ -758,10 +1226,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76643D5-62EC-4DF3-85F2-7E4F76A9A9A4}">
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:L168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="K149" sqref="K149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,7 +2124,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>119</v>
       </c>
@@ -1670,7 +2138,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>72</v>
       </c>
@@ -1684,7 +2152,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>73</v>
       </c>
@@ -1698,7 +2166,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -1712,7 +2180,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>76</v>
       </c>
@@ -1726,7 +2194,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>77</v>
       </c>
@@ -1739,8 +2207,9 @@
       <c r="D70" s="1">
         <v>2400</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="L70" s="1"/>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>79</v>
       </c>
@@ -1754,7 +2223,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>81</v>
       </c>
@@ -1766,6 +2235,1328 @@
       </c>
       <c r="D72" s="1">
         <v>1600</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>124</v>
+      </c>
+      <c r="B73" t="s">
+        <v>125</v>
+      </c>
+      <c r="C73">
+        <v>4</v>
+      </c>
+      <c r="D73" s="1">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>126</v>
+      </c>
+      <c r="B74">
+        <v>1960</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74" s="1">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>127</v>
+      </c>
+      <c r="B75">
+        <v>1947</v>
+      </c>
+      <c r="C75">
+        <v>1</v>
+      </c>
+      <c r="D75">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>128</v>
+      </c>
+      <c r="B76" t="s">
+        <v>129</v>
+      </c>
+      <c r="C76">
+        <v>58</v>
+      </c>
+      <c r="D76">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>130</v>
+      </c>
+      <c r="B77">
+        <v>1992</v>
+      </c>
+      <c r="C77">
+        <v>3</v>
+      </c>
+      <c r="D77">
+        <v>2000</v>
+      </c>
+      <c r="L77" s="1"/>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>131</v>
+      </c>
+      <c r="B78" t="s">
+        <v>132</v>
+      </c>
+      <c r="C78">
+        <v>20</v>
+      </c>
+      <c r="D78">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>133</v>
+      </c>
+      <c r="B79" t="s">
+        <v>132</v>
+      </c>
+      <c r="C79">
+        <v>40</v>
+      </c>
+      <c r="D79">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>134</v>
+      </c>
+      <c r="B80" t="s">
+        <v>135</v>
+      </c>
+      <c r="C80">
+        <v>188</v>
+      </c>
+      <c r="D80" s="1">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>136</v>
+      </c>
+      <c r="B81" t="s">
+        <v>137</v>
+      </c>
+      <c r="C81">
+        <v>515</v>
+      </c>
+      <c r="D81" s="1">
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>138</v>
+      </c>
+      <c r="B82" t="s">
+        <v>139</v>
+      </c>
+      <c r="C82">
+        <v>114</v>
+      </c>
+      <c r="D82">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>140</v>
+      </c>
+      <c r="B83" t="s">
+        <v>141</v>
+      </c>
+      <c r="C83">
+        <v>224</v>
+      </c>
+      <c r="D83">
+        <v>2400</v>
+      </c>
+      <c r="L83" s="1"/>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>142</v>
+      </c>
+      <c r="B84" t="s">
+        <v>143</v>
+      </c>
+      <c r="C84">
+        <v>12</v>
+      </c>
+      <c r="D84">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>144</v>
+      </c>
+      <c r="B85" t="s">
+        <v>145</v>
+      </c>
+      <c r="C85">
+        <v>360</v>
+      </c>
+      <c r="D85">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>146</v>
+      </c>
+      <c r="B86" t="s">
+        <v>16</v>
+      </c>
+      <c r="C86">
+        <v>35</v>
+      </c>
+      <c r="D86">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>147</v>
+      </c>
+      <c r="B87" t="s">
+        <v>148</v>
+      </c>
+      <c r="C87">
+        <v>108</v>
+      </c>
+      <c r="D87">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>149</v>
+      </c>
+      <c r="B88">
+        <v>1971</v>
+      </c>
+      <c r="C88">
+        <v>15</v>
+      </c>
+      <c r="D88">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>150</v>
+      </c>
+      <c r="B89" t="s">
+        <v>151</v>
+      </c>
+      <c r="C89">
+        <v>90</v>
+      </c>
+      <c r="D89">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>152</v>
+      </c>
+      <c r="B90">
+        <v>1967</v>
+      </c>
+      <c r="C90">
+        <v>40</v>
+      </c>
+      <c r="D90">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>153</v>
+      </c>
+      <c r="B91" t="s">
+        <v>154</v>
+      </c>
+      <c r="C91">
+        <v>54</v>
+      </c>
+      <c r="D91">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>155</v>
+      </c>
+      <c r="B92" t="s">
+        <v>156</v>
+      </c>
+      <c r="C92">
+        <v>10</v>
+      </c>
+      <c r="D92">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>157</v>
+      </c>
+      <c r="B93" t="s">
+        <v>16</v>
+      </c>
+      <c r="C93">
+        <v>9</v>
+      </c>
+      <c r="D93">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>158</v>
+      </c>
+      <c r="B94" t="s">
+        <v>100</v>
+      </c>
+      <c r="C94" s="1">
+        <v>1268</v>
+      </c>
+      <c r="D94">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>159</v>
+      </c>
+      <c r="B95" t="s">
+        <v>32</v>
+      </c>
+      <c r="C95">
+        <v>18</v>
+      </c>
+      <c r="D95">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>160</v>
+      </c>
+      <c r="B96" t="s">
+        <v>161</v>
+      </c>
+      <c r="C96">
+        <v>20</v>
+      </c>
+      <c r="D96">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>162</v>
+      </c>
+      <c r="B97" t="s">
+        <v>109</v>
+      </c>
+      <c r="C97">
+        <v>312</v>
+      </c>
+      <c r="D97">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>163</v>
+      </c>
+      <c r="B98" t="s">
+        <v>164</v>
+      </c>
+      <c r="C98" s="1">
+        <v>3982</v>
+      </c>
+      <c r="D98">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>165</v>
+      </c>
+      <c r="B99" t="s">
+        <v>166</v>
+      </c>
+      <c r="C99">
+        <v>123</v>
+      </c>
+      <c r="D99">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>167</v>
+      </c>
+      <c r="B100" t="s">
+        <v>168</v>
+      </c>
+      <c r="C100">
+        <v>9</v>
+      </c>
+      <c r="D100">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>169</v>
+      </c>
+      <c r="B101" t="s">
+        <v>38</v>
+      </c>
+      <c r="C101" s="1">
+        <v>1260</v>
+      </c>
+      <c r="D101">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>170</v>
+      </c>
+      <c r="B102" t="s">
+        <v>25</v>
+      </c>
+      <c r="C102">
+        <v>7</v>
+      </c>
+      <c r="D102">
+        <v>4200</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>171</v>
+      </c>
+      <c r="B103" t="s">
+        <v>172</v>
+      </c>
+      <c r="C103">
+        <v>52</v>
+      </c>
+      <c r="D103">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>173</v>
+      </c>
+      <c r="B104" t="s">
+        <v>174</v>
+      </c>
+      <c r="C104">
+        <v>247</v>
+      </c>
+      <c r="D104">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>175</v>
+      </c>
+      <c r="B105" t="s">
+        <v>176</v>
+      </c>
+      <c r="C105">
+        <v>136</v>
+      </c>
+      <c r="D105">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>177</v>
+      </c>
+      <c r="B106" t="s">
+        <v>48</v>
+      </c>
+      <c r="C106">
+        <v>426</v>
+      </c>
+      <c r="D106">
+        <v>3550</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>178</v>
+      </c>
+      <c r="B107">
+        <v>1980</v>
+      </c>
+      <c r="C107">
+        <v>6</v>
+      </c>
+      <c r="D107">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>179</v>
+      </c>
+      <c r="B108" t="s">
+        <v>180</v>
+      </c>
+      <c r="C108">
+        <v>537</v>
+      </c>
+      <c r="D108">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>181</v>
+      </c>
+      <c r="B109" t="s">
+        <v>182</v>
+      </c>
+      <c r="C109">
+        <v>80</v>
+      </c>
+      <c r="D109">
+        <v>3800</v>
+      </c>
+      <c r="L109" s="1"/>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>183</v>
+      </c>
+      <c r="B110" t="s">
+        <v>184</v>
+      </c>
+      <c r="C110">
+        <v>463</v>
+      </c>
+      <c r="D110">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>185</v>
+      </c>
+      <c r="B111" t="s">
+        <v>186</v>
+      </c>
+      <c r="C111">
+        <v>4</v>
+      </c>
+      <c r="D111">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>187</v>
+      </c>
+      <c r="B112" t="s">
+        <v>188</v>
+      </c>
+      <c r="C112">
+        <v>122</v>
+      </c>
+      <c r="D112">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>189</v>
+      </c>
+      <c r="B113">
+        <v>1995</v>
+      </c>
+      <c r="C113">
+        <v>26</v>
+      </c>
+      <c r="D113">
+        <v>4000</v>
+      </c>
+      <c r="L113" s="1"/>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>190</v>
+      </c>
+      <c r="B114" t="s">
+        <v>191</v>
+      </c>
+      <c r="C114" s="1">
+        <v>2445</v>
+      </c>
+      <c r="D114">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>192</v>
+      </c>
+      <c r="B115" t="s">
+        <v>193</v>
+      </c>
+      <c r="C115">
+        <v>38</v>
+      </c>
+      <c r="D115">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
+        <v>194</v>
+      </c>
+      <c r="B116" t="s">
+        <v>195</v>
+      </c>
+      <c r="C116" s="1">
+        <v>1609</v>
+      </c>
+      <c r="D116">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>196</v>
+      </c>
+      <c r="B117" t="s">
+        <v>197</v>
+      </c>
+      <c r="C117">
+        <v>331</v>
+      </c>
+      <c r="D117">
+        <v>4300</v>
+      </c>
+      <c r="L117" s="1"/>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
+        <v>198</v>
+      </c>
+      <c r="B118" t="s">
+        <v>199</v>
+      </c>
+      <c r="C118" s="1">
+        <v>1109</v>
+      </c>
+      <c r="D118">
+        <v>4150</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>200</v>
+      </c>
+      <c r="B119" t="s">
+        <v>201</v>
+      </c>
+      <c r="C119">
+        <v>76</v>
+      </c>
+      <c r="D119">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>202</v>
+      </c>
+      <c r="B120" t="s">
+        <v>203</v>
+      </c>
+      <c r="C120">
+        <v>204</v>
+      </c>
+      <c r="D120">
+        <v>4300</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>204</v>
+      </c>
+      <c r="B121" t="s">
+        <v>201</v>
+      </c>
+      <c r="C121">
+        <v>37</v>
+      </c>
+      <c r="D121">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>205</v>
+      </c>
+      <c r="B122">
+        <v>2000</v>
+      </c>
+      <c r="C122">
+        <v>1</v>
+      </c>
+      <c r="D122">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>206</v>
+      </c>
+      <c r="B123" t="s">
+        <v>207</v>
+      </c>
+      <c r="C123">
+        <v>478</v>
+      </c>
+      <c r="D123">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>208</v>
+      </c>
+      <c r="B124" t="s">
+        <v>209</v>
+      </c>
+      <c r="C124">
+        <v>123</v>
+      </c>
+      <c r="D124">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>210</v>
+      </c>
+      <c r="B125" t="s">
+        <v>211</v>
+      </c>
+      <c r="C125">
+        <v>30</v>
+      </c>
+      <c r="D125">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>212</v>
+      </c>
+      <c r="B126">
+        <v>1965</v>
+      </c>
+      <c r="C126">
+        <v>15</v>
+      </c>
+      <c r="D126">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>213</v>
+      </c>
+      <c r="B127" t="s">
+        <v>214</v>
+      </c>
+      <c r="C127">
+        <v>47</v>
+      </c>
+      <c r="D127">
+        <v>6600</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>215</v>
+      </c>
+      <c r="B128" t="s">
+        <v>172</v>
+      </c>
+      <c r="C128">
+        <v>14</v>
+      </c>
+      <c r="D128">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>216</v>
+      </c>
+      <c r="B129" t="s">
+        <v>217</v>
+      </c>
+      <c r="C129">
+        <v>86</v>
+      </c>
+      <c r="D129">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>218</v>
+      </c>
+      <c r="B130" t="s">
+        <v>30</v>
+      </c>
+      <c r="C130">
+        <v>150</v>
+      </c>
+      <c r="D130">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>219</v>
+      </c>
+      <c r="B131">
+        <v>1974</v>
+      </c>
+      <c r="C131">
+        <v>15</v>
+      </c>
+      <c r="D131">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>220</v>
+      </c>
+      <c r="B132" t="s">
+        <v>221</v>
+      </c>
+      <c r="C132">
+        <v>187</v>
+      </c>
+      <c r="D132">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>222</v>
+      </c>
+      <c r="B133" t="s">
+        <v>223</v>
+      </c>
+      <c r="C133">
+        <v>132</v>
+      </c>
+      <c r="D133">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>224</v>
+      </c>
+      <c r="B134" t="s">
+        <v>225</v>
+      </c>
+      <c r="C134">
+        <v>4</v>
+      </c>
+      <c r="D134">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>226</v>
+      </c>
+      <c r="B135" t="s">
+        <v>50</v>
+      </c>
+      <c r="C135">
+        <v>31</v>
+      </c>
+      <c r="D135">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>227</v>
+      </c>
+      <c r="B136" t="s">
+        <v>228</v>
+      </c>
+      <c r="C136">
+        <v>26</v>
+      </c>
+      <c r="D136">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>229</v>
+      </c>
+      <c r="B137" t="s">
+        <v>186</v>
+      </c>
+      <c r="C137">
+        <v>30</v>
+      </c>
+      <c r="D137">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>230</v>
+      </c>
+      <c r="B138">
+        <v>1988</v>
+      </c>
+      <c r="C138">
+        <v>25</v>
+      </c>
+      <c r="D138">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>231</v>
+      </c>
+      <c r="B139" t="s">
+        <v>232</v>
+      </c>
+      <c r="C139">
+        <v>60</v>
+      </c>
+      <c r="D139">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>233</v>
+      </c>
+      <c r="B140" t="s">
+        <v>50</v>
+      </c>
+      <c r="C140">
+        <v>64</v>
+      </c>
+      <c r="D140">
+        <v>3800</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>234</v>
+      </c>
+      <c r="B141" t="s">
+        <v>235</v>
+      </c>
+      <c r="C141">
+        <v>72</v>
+      </c>
+      <c r="D141">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>236</v>
+      </c>
+      <c r="B142" t="s">
+        <v>237</v>
+      </c>
+      <c r="C142">
+        <v>83</v>
+      </c>
+      <c r="D142">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>238</v>
+      </c>
+      <c r="B143">
+        <v>1989</v>
+      </c>
+      <c r="C143">
+        <v>2</v>
+      </c>
+      <c r="D143">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>239</v>
+      </c>
+      <c r="B144" t="s">
+        <v>241</v>
+      </c>
+      <c r="C144">
+        <v>23</v>
+      </c>
+      <c r="D144">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>240</v>
+      </c>
+      <c r="B145" t="s">
+        <v>244</v>
+      </c>
+      <c r="C145">
+        <v>12</v>
+      </c>
+      <c r="D145">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>242</v>
+      </c>
+      <c r="B146" t="s">
+        <v>243</v>
+      </c>
+      <c r="C146">
+        <v>40</v>
+      </c>
+      <c r="D146">
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>245</v>
+      </c>
+      <c r="B147" t="s">
+        <v>246</v>
+      </c>
+      <c r="C147">
+        <v>233</v>
+      </c>
+      <c r="D147">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>247</v>
+      </c>
+      <c r="B148" t="s">
+        <v>248</v>
+      </c>
+      <c r="C148">
+        <v>7</v>
+      </c>
+      <c r="D148">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>249</v>
+      </c>
+      <c r="B149" t="s">
+        <v>250</v>
+      </c>
+      <c r="C149">
+        <v>155</v>
+      </c>
+      <c r="D149">
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>251</v>
+      </c>
+      <c r="B150" t="s">
+        <v>252</v>
+      </c>
+      <c r="C150">
+        <v>10</v>
+      </c>
+      <c r="D150">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>253</v>
+      </c>
+      <c r="B151" t="s">
+        <v>254</v>
+      </c>
+      <c r="C151">
+        <v>85</v>
+      </c>
+      <c r="D151">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>255</v>
+      </c>
+      <c r="B152" t="s">
+        <v>256</v>
+      </c>
+      <c r="C152">
+        <v>16</v>
+      </c>
+      <c r="D152">
+        <v>1650</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>257</v>
+      </c>
+      <c r="B153" t="s">
+        <v>248</v>
+      </c>
+      <c r="C153">
+        <v>3</v>
+      </c>
+      <c r="D153">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>258</v>
+      </c>
+      <c r="B154" t="s">
+        <v>259</v>
+      </c>
+      <c r="C154">
+        <v>8</v>
+      </c>
+      <c r="D154">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>260</v>
+      </c>
+      <c r="B155">
+        <v>1988</v>
+      </c>
+      <c r="C155">
+        <v>6</v>
+      </c>
+      <c r="D155">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>261</v>
+      </c>
+      <c r="B156" t="s">
+        <v>262</v>
+      </c>
+      <c r="D156">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>263</v>
+      </c>
+      <c r="B157" t="s">
+        <v>264</v>
+      </c>
+      <c r="D157">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>265</v>
+      </c>
+      <c r="B158">
+        <v>1990</v>
+      </c>
+      <c r="C158">
+        <v>20</v>
+      </c>
+      <c r="D158">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>266</v>
+      </c>
+      <c r="D159">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>267</v>
+      </c>
+      <c r="B160" t="s">
+        <v>268</v>
+      </c>
+      <c r="C160">
+        <v>80</v>
+      </c>
+      <c r="D160">
+        <v>2650</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>269</v>
+      </c>
+      <c r="D161">
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>270</v>
+      </c>
+      <c r="B162">
+        <v>2009</v>
+      </c>
+      <c r="D162">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>271</v>
+      </c>
+      <c r="B163">
+        <v>2009</v>
+      </c>
+      <c r="C163">
+        <v>4</v>
+      </c>
+      <c r="D163">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>272</v>
+      </c>
+      <c r="B164">
+        <v>2009</v>
+      </c>
+      <c r="D164">
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>273</v>
+      </c>
+      <c r="B165">
+        <v>2013</v>
+      </c>
+      <c r="C165">
+        <v>130</v>
+      </c>
+      <c r="D165">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>274</v>
+      </c>
+      <c r="B166" t="s">
+        <v>275</v>
+      </c>
+      <c r="C166">
+        <v>63</v>
+      </c>
+      <c r="D166">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>276</v>
+      </c>
+      <c r="B167" t="s">
+        <v>277</v>
+      </c>
+      <c r="D167">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>278</v>
+      </c>
+      <c r="B168" t="s">
+        <v>279</v>
+      </c>
+      <c r="C168">
+        <v>20</v>
+      </c>
+      <c r="D168">
+        <v>1870</v>
       </c>
     </row>
   </sheetData>

</xml_diff>